<commit_message>
update RIZAP CRM issues.xls
</commit_message>
<xml_diff>
--- a/RIZAP Issues/RIZAP CRM issues.xlsx
+++ b/RIZAP Issues/RIZAP CRM issues.xlsx
@@ -1376,6 +1376,128 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>[2021-09-16 Paul Kang]:
+Reverve the last result of customerPaidAmont at the last row of the same contract. Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2021-07-12 Paul Kang:]
+Benjamin confirmed the definitation of "Refund amount". </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Benjamin replied the definitioons on 7/22.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[2021-08-18 Paul Kang]:
+Instead of CSV export file, uCare implements Sessions data in the Web tools. There are 76 columns, under development. Under developing.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[2021-08-19 Meeting]:
+Benjamin will arrange an afternoon to uCare to discuss the defininations.
+[2021-08-26 Paul and Benjamin on-line discussion]:
+1. Remove "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>退費堂數</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">" Session.
+2. Disuss the YearContract definition.
+3. uCare to finish the Web-tool YearContract.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[2021-09-01 Paul Kang]:
+Web-tools Alpha2 released for Session and YearContract</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[2021-09-16 Paul Kang]:
+Multiple payments listed in different rows, but only the first row has full data, the rest rows only have didderent payment data. Done</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>[Type: Information]
 1. If the fiscal year of RIZAP USA also starts from 1st of April?
@@ -1410,37 +1532,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-[2021-09-01]
-5. What is the tax rate in LA and Hawaii?</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[2021-09-16 Paul Kang]:
-Reverve the last result of customerPaidAmont at the last row of the same contract. Done</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[2021-07-12 Paul Kang:]
-Benjamin confirmed the definitation of "Refund amount". </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Benjamin replied the definitioons on 7/22.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 
 </t>
     </r>
     <r>
@@ -1450,90 +1541,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>[2021-08-18 Paul Kang]:
-Instead of CSV export file, uCare implements Sessions data in the Web tools. There are 76 columns, under development. Under developing.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[2021-08-19 Meeting]:
-Benjamin will arrange an afternoon to uCare to discuss the defininations.
-[2021-08-26 Paul and Benjamin on-line discussion]:
-1. Remove "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="細明體"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>退費堂數</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">" Session.
-2. Disuss the YearContract definition.
-3. uCare to finish the Web-tool YearContract.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[2021-09-01 Paul Kang]:
-Web-tools Alpha2 released for Session and YearContract</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[2021-09-16 Paul Kang]:
-Multiple payments listed in different rows, but only the first row has full data, the rest rows only have didderent payment data. Done</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
+      <t>[2021-09-01]
+5. What is the tax rate in LA and Hawaii?</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1554,7 +1563,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -1613,7 +1622,8 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-[based on 10/7 MTG] Before the English translation is completed, uCare to set up a virtual machine server for Santa Monica store. With the existing language condition as a beta CRM system for training first, due by 10/14.</t>
+[based on 10/7 MTG] Before the English translation is completed, uCare to set up a virtual machine server for Santa Monica store. With the existing language condition as a beta CRM system for training first, due by 10/14.
+6. [2021-10-14] Inquery form API for Santa Monica store (due: 10/21)</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2261,14 +2271,14 @@
         <v>12</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C7" s="5"/>
       <c r="F7" s="17"/>
       <c r="G7" s="39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="24" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.45">
@@ -2340,7 +2350,7 @@
         <v>17</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="F11" s="39" t="s">
         <v>283</v>

</xml_diff>